<commit_message>
Mejoras en diagramas de flujo y genero players_turn.py
</commit_message>
<xml_diff>
--- a/Diagramas de flujo.xlsx
+++ b/Diagramas de flujo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin\Desktop\python\pig game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6855AD63-A714-471F-91EA-305DE4CAE494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3691AE-7829-442B-997B-57E28B7F4C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F961905F-5879-4769-BFBC-EBDC8ACCEC7A}"/>
+    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{F961905F-5879-4769-BFBC-EBDC8ACCEC7A}"/>
   </bookViews>
   <sheets>
     <sheet name="player's_turn" sheetId="1" r:id="rId1"/>
@@ -93,13 +93,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>133351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>13607</xdr:rowOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>33619</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -114,8 +114,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5250996" y="2228850"/>
-          <a:ext cx="6916511" cy="5785757"/>
+          <a:off x="5193366" y="2228851"/>
+          <a:ext cx="6837269" cy="5615268"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -383,7 +383,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="es-AR" sz="1100"/>
-            <a:t>Play</a:t>
+            <a:t>Roll</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="es-AR" sz="1100" baseline="0"/>
@@ -1818,15 +1818,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>238124</xdr:colOff>
+      <xdr:colOff>238125</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>133351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>136751</xdr:colOff>
+      <xdr:colOff>140354</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>121378</xdr:rowOff>
+      <xdr:rowOff>121377</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1844,13 +1844,13 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipH="1">
-          <a:off x="6361338" y="2228851"/>
-          <a:ext cx="2347913" cy="7417527"/>
+          <a:off x="6289301" y="2228851"/>
+          <a:ext cx="2322700" cy="7417526"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector4">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -62822"/>
-            <a:gd name="adj2" fmla="val 105833"/>
+            <a:gd name="adj1" fmla="val -57026"/>
+            <a:gd name="adj2" fmla="val 103082"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -1883,9 +1883,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>136752</xdr:colOff>
+      <xdr:colOff>140354</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>133351</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1903,8 +1903,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8701768" y="1524000"/>
-          <a:ext cx="7484" cy="704850"/>
+          <a:off x="8600915" y="1524000"/>
+          <a:ext cx="11086" cy="704851"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2081,7 +2081,7 @@
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 87143"/>
+            <a:gd name="adj1" fmla="val 95509"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -2108,15 +2108,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>507139</xdr:colOff>
+      <xdr:colOff>503537</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:rowOff>133351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>136752</xdr:colOff>
+      <xdr:colOff>140354</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:rowOff>144781</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2134,12 +2134,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1" flipV="1">
-          <a:off x="7684498" y="1787026"/>
-          <a:ext cx="582931" cy="1466577"/>
+          <a:off x="7594451" y="1794231"/>
+          <a:ext cx="582930" cy="1452170"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 28477"/>
+            <a:gd name="adj1" fmla="val -39216"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -3854,8 +3854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C35AD5-9F1F-42AF-88E9-E1E590FB77C2}">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z27" sqref="Z27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Cambio players_turn.py por roll_dice.py, mejoro diagramas de flujo y empiezo con el main.py
</commit_message>
<xml_diff>
--- a/Diagramas de flujo.xlsx
+++ b/Diagramas de flujo.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin\Desktop\python\pig game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3691AE-7829-442B-997B-57E28B7F4C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B4E86C-66F6-427B-B1D8-514D6B7C0C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{F961905F-5879-4769-BFBC-EBDC8ACCEC7A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F961905F-5879-4769-BFBC-EBDC8ACCEC7A}"/>
   </bookViews>
   <sheets>
-    <sheet name="player's_turn" sheetId="1" r:id="rId1"/>
+    <sheet name="roll_dice" sheetId="1" r:id="rId1"/>
     <sheet name="General flow" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -91,15 +91,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
+      <xdr:colOff>352426</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>133351</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>33619</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>11207</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>22411</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -114,8 +114,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5193366" y="2228851"/>
-          <a:ext cx="6837269" cy="5615268"/>
+          <a:off x="5193367" y="2228850"/>
+          <a:ext cx="5709958" cy="5794561"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -149,15 +149,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>316231</xdr:colOff>
+      <xdr:colOff>305025</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>21517</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>74519</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>144781</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>172011</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -172,8 +172,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6412231" y="1097281"/>
-          <a:ext cx="1598294" cy="340994"/>
+          <a:off x="6356201" y="2498017"/>
+          <a:ext cx="1584847" cy="340994"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -211,14 +211,14 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>559</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>10084</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -233,8 +233,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6400800" y="2409824"/>
-          <a:ext cx="1609725" cy="962025"/>
+          <a:off x="6355976" y="3048559"/>
+          <a:ext cx="1596278" cy="962025"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartDecision">
           <a:avLst/>
@@ -272,14 +272,14 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>59056</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>92670</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>81239</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -294,8 +294,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6324600" y="3678556"/>
-          <a:ext cx="1762125" cy="369569"/>
+          <a:off x="6279776" y="4283670"/>
+          <a:ext cx="1748678" cy="369569"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -334,13 +334,13 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:rowOff>73398</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:rowOff>82923</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -355,8 +355,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6410325" y="5553074"/>
-          <a:ext cx="1609725" cy="962025"/>
+          <a:off x="6365501" y="6550398"/>
+          <a:ext cx="1596278" cy="962025"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartDecision">
           <a:avLst/>
@@ -398,15 +398,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>500063</xdr:colOff>
+      <xdr:colOff>492331</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>172011</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>497821</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>505778</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:rowOff>559</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -423,9 +423,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="7205663" y="2200275"/>
-          <a:ext cx="5715" cy="209549"/>
+        <a:xfrm>
+          <a:off x="7148625" y="2839011"/>
+          <a:ext cx="5490" cy="209548"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -454,15 +454,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>500063</xdr:colOff>
+      <xdr:colOff>497821</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>10084</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>497821</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>500063</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>59056</xdr:rowOff>
+      <xdr:rowOff>92670</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -480,8 +480,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7205663" y="3371849"/>
-          <a:ext cx="0" cy="306707"/>
+          <a:off x="7154115" y="4010584"/>
+          <a:ext cx="0" cy="273086"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -510,15 +510,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
+      <xdr:colOff>305025</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1515</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>124779</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>316231</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>128588</xdr:rowOff>
+      <xdr:rowOff>173412</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -535,13 +535,13 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="10800000" flipH="1">
-          <a:off x="6437539" y="2982279"/>
-          <a:ext cx="1906" cy="4004309"/>
+        <a:xfrm rot="10800000">
+          <a:off x="6356201" y="2668515"/>
+          <a:ext cx="9300" cy="4362897"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -34838877"/>
+            <a:gd name="adj1" fmla="val 7377785"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -690,14 +690,14 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>40006</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>107241</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>95810</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -712,8 +712,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8782050" y="2707006"/>
-          <a:ext cx="1762125" cy="369569"/>
+          <a:off x="8719297" y="3345741"/>
+          <a:ext cx="1748678" cy="369569"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -756,14 +756,14 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>100572</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>34291</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>101526</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -781,8 +781,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8010525" y="2890837"/>
-          <a:ext cx="771525" cy="954"/>
+          <a:off x="7952254" y="3529572"/>
+          <a:ext cx="767043" cy="954"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -808,78 +808,12 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>127092</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>115661</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="33" name="Rectangle 32">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA132C15-D83A-629D-74BE-0C553777F33B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6361339" y="9461592"/>
-          <a:ext cx="1770290" cy="369569"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-AR" sz="1100"/>
-            <a:t>player id =</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
-            <a:t> player id + 1</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-AR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="378758" cy="264560"/>
     <xdr:sp macro="" textlink="">
@@ -895,7 +829,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8181975" y="2667000"/>
+          <a:off x="8123704" y="3305735"/>
           <a:ext cx="378758" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -936,8 +870,8 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152960</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="350096" cy="264560"/>
     <xdr:sp macro="" textlink="">
@@ -953,7 +887,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7200900" y="3324225"/>
+          <a:off x="7151594" y="3962960"/>
           <a:ext cx="350096" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1050,77 +984,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>108857</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>149679</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="49" name="Flowchart: Process 48">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F49FFDEE-6995-1F0D-5586-8EEB8D544269}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8069036" y="1238250"/>
-          <a:ext cx="1265464" cy="285750"/>
-        </a:xfrm>
-        <a:prstGeom prst="flowChartProcess">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-AR" sz="1100"/>
-            <a:t>player id = 1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:rowOff>189379</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>542924</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>8404</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1135,8 +1008,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5953125" y="4324349"/>
-          <a:ext cx="2514599" cy="962025"/>
+          <a:off x="5912784" y="5332879"/>
+          <a:ext cx="2496669" cy="962025"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartDecision">
           <a:avLst/>
@@ -1178,15 +1051,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>500063</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>497821</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>81239</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:colOff>497821</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>47847</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1199,13 +1072,13 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="5" idx="2"/>
-          <a:endCxn id="62" idx="0"/>
+          <a:endCxn id="1113" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7205663" y="4048125"/>
-          <a:ext cx="4762" cy="276224"/>
+          <a:off x="7154115" y="4653239"/>
+          <a:ext cx="0" cy="157108"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1235,14 +1108,14 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>8404</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>509588</xdr:colOff>
+      <xdr:colOff>507346</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:rowOff>73398</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1260,8 +1133,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7210425" y="5286374"/>
-          <a:ext cx="4763" cy="266700"/>
+          <a:off x="7161119" y="6294904"/>
+          <a:ext cx="2521" cy="255494"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1292,7 +1165,7 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>172011</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="350096" cy="264560"/>
     <xdr:sp macro="" textlink="">
@@ -1308,7 +1181,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7210425" y="5248275"/>
+          <a:off x="7161119" y="6268011"/>
           <a:ext cx="350096" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1347,77 +1220,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>68036</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>150224</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>1361</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>138793</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="71" name="Rectangle 70">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{746C40D0-25E4-AAE1-2302-5DE5E6C7DE72}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13539107" y="6436724"/>
-          <a:ext cx="1770290" cy="369569"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-AR" sz="1100"/>
-            <a:t>Show winner</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>180654</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>98892</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>542924</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>340859</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>150224</xdr:rowOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>99685</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1429,17 +1241,20 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
           <a:stCxn id="62" idx="3"/>
-          <a:endCxn id="71" idx="0"/>
+          <a:endCxn id="1124" idx="3"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8503103" y="5757862"/>
-          <a:ext cx="5921149" cy="678862"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
+        <a:xfrm flipH="1">
+          <a:off x="8047183" y="5813892"/>
+          <a:ext cx="362270" cy="3048793"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -830225"/>
+          </a:avLst>
         </a:prstGeom>
         <a:ln>
           <a:tailEnd type="triangle"/>
@@ -1522,23 +1337,139 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>507346</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>82923</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>516550</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>105400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="123" name="Straight Arrow Connector 122">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5674E6B-93D9-71D9-D022-AC0196D059C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="6" idx="2"/>
+          <a:endCxn id="1124" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7163640" y="7512423"/>
+          <a:ext cx="9204" cy="1165477"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>516550</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>95810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>516871</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>105400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="1050" name="Connector: Elbow 1049">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C0E6BBC-B537-D250-09BF-1ACEEBB5629B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="28" idx="2"/>
+          <a:endCxn id="1124" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5901945" y="4986209"/>
+          <a:ext cx="4962590" cy="2420792"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 82065"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>122464</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>47847</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>299357</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>36416</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="107" name="Flowchart: Decision 106">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14B1598F-7C2E-33F0-BB8E-46D7C8CB36D7}"/>
+        <xdr:cNvPr id="1113" name="Rectangle 1112">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D92EF8AA-69E8-6744-CF6E-681FF9AD4861}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1546,10 +1477,10 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6245678" y="8315324"/>
-          <a:ext cx="2013858" cy="962025"/>
-        </a:xfrm>
-        <a:prstGeom prst="flowChartDecision">
+          <a:off x="6279776" y="4810347"/>
+          <a:ext cx="1748678" cy="369569"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -1574,11 +1505,11 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="es-AR" sz="1100"/>
-            <a:t>Last</a:t>
+            <a:t>"Score</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="es-AR" sz="1100" baseline="0"/>
-            <a:t> player?</a:t>
+            <a:t> for this round + global score"</a:t>
           </a:r>
           <a:endParaRPr lang="es-AR" sz="1100"/>
         </a:p>
@@ -1588,41 +1519,38 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>299357</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>129268</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>497821</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>36416</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>189379</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="112" name="Connector: Elbow 111">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2979EB1-1B28-570A-EDFB-C0B735CB4072}"/>
+        <xdr:cNvPr id="1116" name="Straight Arrow Connector 1115">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CF00B03-6F3B-0737-52F2-6CE468D35513}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="107" idx="3"/>
-          <a:endCxn id="49" idx="0"/>
+          <a:stCxn id="1113" idx="2"/>
+          <a:endCxn id="62" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="8259536" y="1238250"/>
-          <a:ext cx="442232" cy="7558087"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector4">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 1030154"/>
-            <a:gd name="adj2" fmla="val 103025"/>
-          </a:avLst>
+        <a:xfrm>
+          <a:off x="7154115" y="5179916"/>
+          <a:ext cx="7004" cy="152963"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
         </a:prstGeom>
         <a:ln>
           <a:tailEnd type="triangle"/>
@@ -1645,366 +1573,25 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>247329</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>105400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>327933</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>157843</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="378758" cy="264560"/>
+      <xdr:colOff>180654</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>93969</xdr:rowOff>
+    </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="115" name="TextBox 114">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CF97181-40EF-2C17-6571-EE9FCCAA2742}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8288112" y="8539843"/>
-          <a:ext cx="378758" cy="264560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-AR" sz="1100"/>
-            <a:t>Yes</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>510948</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>517071</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="123" name="Straight Arrow Connector 122">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5674E6B-93D9-71D9-D022-AC0196D059C5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="6" idx="2"/>
-          <a:endCxn id="107" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7246484" y="7467599"/>
-          <a:ext cx="6123" cy="847725"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>510948</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>517071</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>127092</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="1024" name="Straight Arrow Connector 1023">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1019E1C2-D5F4-C486-2AB7-0DE00B884BDA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="107" idx="2"/>
-          <a:endCxn id="33" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="7246484" y="9277349"/>
-          <a:ext cx="6123" cy="184243"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>133351</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>140354</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>121377</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="1028" name="Connector: Elbow 1027">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B12A4B13-44AE-CBAD-2640-B9BE0ECA6A00}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="33" idx="1"/>
-          <a:endCxn id="24" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000" flipH="1">
-          <a:off x="6289301" y="2228851"/>
-          <a:ext cx="2322700" cy="7417526"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector4">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -57026"/>
-            <a:gd name="adj2" fmla="val 103082"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>129268</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>140354</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>133351</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="1036" name="Straight Arrow Connector 1035">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32EC2009-A257-5651-1A03-226266A09E7E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="49" idx="2"/>
-          <a:endCxn id="24" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8600915" y="1524000"/>
-          <a:ext cx="11086" cy="704851"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>129267</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>176893</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>129268</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="1041" name="Straight Arrow Connector 1040">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4438A4F4-4191-CF67-515C-CA9D93D745DE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="1046" idx="2"/>
-          <a:endCxn id="49" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8701767" y="748393"/>
-          <a:ext cx="1" cy="489857"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>108856</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>81643</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>149678</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>176893</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1046" name="Flowchart: Process 1045">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97CECFA8-53D3-54C5-2F22-F2247FE4F415}"/>
+        <xdr:cNvPr id="1124" name="Rectangle 1123">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB2825AD-6152-A078-6030-3805999FFB05}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2012,10 +1599,10 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8069035" y="462643"/>
-          <a:ext cx="1265464" cy="285750"/>
-        </a:xfrm>
-        <a:prstGeom prst="flowChartProcess">
+          <a:off x="6298505" y="8677900"/>
+          <a:ext cx="1748678" cy="369569"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -2040,127 +1627,16 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="es-AR" sz="1100"/>
-            <a:t>General flow</a:t>
+            <a:t>return</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
+            <a:t> global_score</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-AR" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>517072</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>520475</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>123823</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="1050" name="Connector: Elbow 1049">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C0E6BBC-B537-D250-09BF-1ACEEBB5629B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="28" idx="2"/>
-          <a:endCxn id="107" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="6335827" y="4945855"/>
-          <a:ext cx="4286249" cy="2452688"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 95509"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>503537</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>133351</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>140354</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>144781</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="1065" name="Connector: Elbow 1064">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACF589BE-9532-6DB3-8FB3-E158E7F3C58F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="24" idx="0"/>
-          <a:endCxn id="3" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000" flipH="1" flipV="1">
-          <a:off x="7594451" y="1794231"/>
-          <a:ext cx="582930" cy="1452170"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -39216"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2172,13 +1648,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2231,13 +1707,13 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>561975</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>16002</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>111252</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2252,7 +1728,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7877175" y="285750"/>
+          <a:off x="7877175" y="190500"/>
           <a:ext cx="914400" cy="301752"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartTerminator">
@@ -2290,15 +1766,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>571501</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>542926</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2313,7 +1789,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7629525" y="1990725"/>
+          <a:off x="7600950" y="3000375"/>
           <a:ext cx="1476376" cy="276225"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
@@ -2355,15 +1831,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2379,7 +1855,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7324725" y="2533650"/>
+          <a:off x="7305675" y="3486150"/>
           <a:ext cx="2076450" cy="800100"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartDecision">
@@ -2417,14 +1893,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>571501</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>33338</xdr:rowOff>
+      <xdr:colOff>542926</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>90488</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2443,12 +1919,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="9105901" y="2128838"/>
-          <a:ext cx="295274" cy="804862"/>
+          <a:off x="9077326" y="3138488"/>
+          <a:ext cx="304799" cy="747712"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -119356"/>
+            <a:gd name="adj1" fmla="val -140625"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -2476,7 +1952,7 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="350096" cy="264560"/>
@@ -2533,14 +2009,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>581026</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:colOff>552451</xdr:colOff>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2556,7 +2032,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7639050" y="3848100"/>
+          <a:off x="7610475" y="4800600"/>
           <a:ext cx="1476376" cy="276225"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
@@ -2593,15 +2069,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2617,7 +2093,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7334250" y="4381500"/>
+          <a:off x="7305675" y="5334000"/>
           <a:ext cx="2076450" cy="800100"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartDecision">
@@ -2654,16 +2130,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>19049</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>93346</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>102870</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>409574</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2682,13 +2158,13 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipH="1">
-          <a:off x="7334249" y="1045846"/>
-          <a:ext cx="1000125" cy="3735705"/>
+          <a:off x="7305675" y="864870"/>
+          <a:ext cx="1028700" cy="4869180"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector4">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -86667"/>
-            <a:gd name="adj2" fmla="val 107343"/>
+            <a:gd name="adj1" fmla="val -93518"/>
+            <a:gd name="adj2" fmla="val 105634"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -2714,15 +2190,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>35052</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2738,7 +2214,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7924800" y="6210300"/>
+          <a:off x="7896225" y="7162800"/>
           <a:ext cx="914400" cy="301752"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartTerminator">
@@ -2776,14 +2252,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>581026</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:colOff>552451</xdr:colOff>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2799,7 +2275,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7639050" y="5505450"/>
+          <a:off x="7610475" y="6457950"/>
           <a:ext cx="1476376" cy="276225"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
@@ -2838,7 +2314,7 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="378758" cy="264560"/>
@@ -2895,14 +2371,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>452438</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:colOff>423863</xdr:colOff>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2921,7 +2397,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8372475" y="5181600"/>
+          <a:off x="8343900" y="6134100"/>
           <a:ext cx="4763" cy="323850"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -2951,14 +2427,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>452438</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:colOff>423863</xdr:colOff>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2977,7 +2453,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8377238" y="5781675"/>
+          <a:off x="8348663" y="6734175"/>
           <a:ext cx="4762" cy="428625"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -3008,7 +2484,7 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="350096" cy="264560"/>
@@ -3065,14 +2541,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>414338</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>442913</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3090,9 +2566,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="8362950" y="2266950"/>
-          <a:ext cx="4763" cy="266700"/>
+        <a:xfrm>
+          <a:off x="8339138" y="3276600"/>
+          <a:ext cx="4762" cy="209550"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3121,14 +2597,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>452438</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:colOff>423863</xdr:colOff>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3147,8 +2623,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8362950" y="3333750"/>
-          <a:ext cx="14288" cy="514350"/>
+          <a:off x="8343900" y="4286250"/>
+          <a:ext cx="4763" cy="514350"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3177,14 +2653,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>452438</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:colOff>423863</xdr:colOff>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3203,7 +2679,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="8372475" y="4124325"/>
+          <a:off x="8343900" y="5076825"/>
           <a:ext cx="4763" cy="257175"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -3234,7 +2710,7 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="378758" cy="264560"/>
@@ -3292,7 +2768,7 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1344342" cy="264560"/>
@@ -3350,14 +2826,14 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>16002</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>111252</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>93345</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>102870</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3376,8 +2852,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8334375" y="587502"/>
-          <a:ext cx="0" cy="458343"/>
+          <a:off x="8334375" y="492252"/>
+          <a:ext cx="0" cy="372618"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3405,73 +2881,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>414338</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="56" name="Straight Arrow Connector 55">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDAB7CF7-4EC8-3AB6-D37C-4A563F7FB20C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:cxnSpLocks/>
-          <a:stCxn id="65" idx="2"/>
-          <a:endCxn id="46" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8334375" y="1457325"/>
-          <a:ext cx="4763" cy="381000"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3486,7 +2905,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7591425" y="1000125"/>
+          <a:off x="7591425" y="819150"/>
           <a:ext cx="1485900" cy="457200"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartManualInput">
@@ -3552,6 +2971,526 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="82" name="Flowchart: Decision 81">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB82434B-2C63-AB2E-061B-6C539752C501}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7296150" y="1438275"/>
+          <a:ext cx="2076450" cy="1009650"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>input is not a number?</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="87" name="Straight Arrow Connector 86">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26CD8363-7B33-56FE-A22E-4E33CD23A95B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="65" idx="2"/>
+          <a:endCxn id="82" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8334375" y="1276350"/>
+          <a:ext cx="0" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>380999</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="95" name="Flowchart: Process 94">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA672CD7-CC3D-CD62-8A8B-FF38C88414DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10134599" y="1809750"/>
+          <a:ext cx="1943101" cy="276225"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartProcess">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>"Invalid entry, try again"</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>42863</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="97" name="Connector: Elbow 96">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA7A8EB9-2A24-26F8-1EB1-B7D10126D8D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="95" idx="3"/>
+          <a:endCxn id="65" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="9077325" y="1047750"/>
+          <a:ext cx="3000375" cy="900113"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -7619"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>380999</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>42863</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="99" name="Straight Arrow Connector 98">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E671037A-9AF9-7674-DDE2-91D2E005CA58}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="82" idx="3"/>
+          <a:endCxn id="95" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9372600" y="1943100"/>
+          <a:ext cx="761999" cy="4763"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>414338</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="101" name="Straight Arrow Connector 100">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29BFDAF4-735F-AC19-D8AA-66C122C7B99E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="82" idx="2"/>
+          <a:endCxn id="46" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8334375" y="2447925"/>
+          <a:ext cx="4763" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>414338</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>414338</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="106" name="Straight Arrow Connector 105">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5909D3C-AAF7-D60F-E398-553503378215}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="46" idx="0"/>
+          <a:endCxn id="5" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8339138" y="2790825"/>
+          <a:ext cx="0" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="350096" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="109" name="TextBox 108">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24250300-90B6-39D3-C1C0-ACD21878746E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8324850" y="2428875"/>
+          <a:ext cx="350096" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>No</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="378758" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="110" name="TextBox 109">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{837407DD-B562-ADA5-7433-5CA038C45637}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9534525" y="1685925"/>
+          <a:ext cx="378758" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>Yes</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3855,7 +3794,7 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z27" sqref="Z27"/>
+      <selection activeCell="U38" sqref="U38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3877,14 +3816,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{372A6B47-11E3-4BB2-859D-A356626AFE6D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Termino diagramas de flujo y agrego funcionalidad play again cuando el juego termina.
</commit_message>
<xml_diff>
--- a/Diagramas de flujo.xlsx
+++ b/Diagramas de flujo.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin\Desktop\python\pig game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A02550-9CA5-4309-9695-EF3654CF98FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A903EFD8-FB5D-474B-ADD4-30842FE109FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{F961905F-5879-4769-BFBC-EBDC8ACCEC7A}"/>
+    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F961905F-5879-4769-BFBC-EBDC8ACCEC7A}"/>
   </bookViews>
   <sheets>
     <sheet name="roll_dice" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1982,6 +1983,2072 @@
           <a:r>
             <a:rPr lang="es-AR" sz="1100"/>
             <a:t>Yes</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>257174</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Flowchart: Manual Input 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A5D03A0-6B8C-C4A5-52F9-55FE8779E0CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705599" y="904875"/>
+          <a:ext cx="1476375" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartManualInput">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>Number of players?</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>257176</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CC9819E-5646-4569-D1D8-855C27F12AA8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705600" y="2552700"/>
+          <a:ext cx="1476376" cy="295275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>Roll dice for player</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>257174</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EC22953-E204-8FDF-8DA0-654C257351C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6095999" y="1666875"/>
+          <a:ext cx="2695575" cy="428625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>Set global scores to 0 for each player</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>12573</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Flowchart: Decision 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7229502F-1A70-0CA0-9420-FB6BB299654D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6724650" y="3209925"/>
+          <a:ext cx="1428750" cy="612648"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>Dice = 0?</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>128588</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E10BAB99-907F-7241-A94E-88C7CB9519A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="2"/>
+          <a:endCxn id="5" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7439025" y="2847975"/>
+          <a:ext cx="4763" cy="361950"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="378758" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="TextBox 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E9E0DB6-7608-EAFB-F4AA-83FF332601DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7086600" y="3810000"/>
+          <a:ext cx="378758" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>Yes</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>12573</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9CC3A80-FD7A-C3E5-D0A0-51A4B77FF3B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="5" idx="2"/>
+          <a:endCxn id="33" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7439025" y="3822573"/>
+          <a:ext cx="0" cy="368427"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="Flowchart: Decision 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FE2385D-5789-5CE6-9C8C-32E775234556}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9858374" y="3067049"/>
+          <a:ext cx="2857501" cy="904875"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>Player's global score &gt;=</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
+            <a:t> threshold?</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-AR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>87249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Straight Arrow Connector 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93FABA25-AE34-4CF8-9A3A-09210CCFCCC9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="3"/>
+          <a:endCxn id="23" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8153400" y="3516249"/>
+          <a:ext cx="1704974" cy="3238"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="350096" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="TextBox 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF66B114-0552-C55D-18EA-47B9DF461BC5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8267700" y="3276600"/>
+          <a:ext cx="350096" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>No</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>257176</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>33338</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Connector: Elbow 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42F9CD39-E4D8-B901-6AAA-06C3BAD7C06E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="23" idx="3"/>
+          <a:endCxn id="3" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8181976" y="2700338"/>
+          <a:ext cx="4533899" cy="819149"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -13866"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="350096" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="TextBox 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AC577AA-8D7B-D7EB-7797-99E88DBD2CFB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12763500" y="3295650"/>
+          <a:ext cx="350096" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>No</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>485774</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="Flowchart: Decision 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{103791A7-E340-DE83-684B-ABFC2291298D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6467475" y="4191000"/>
+          <a:ext cx="1943099" cy="990600"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>Last</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
+            <a:t> player in round?</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-AR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>257176</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="Rectangle 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77A35326-72D4-79BF-6F12-043ACF2032DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705600" y="5438775"/>
+          <a:ext cx="1476376" cy="295275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>Next player's turn</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>128588</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="50" name="Straight Arrow Connector 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B158BAE-E5C6-9092-A86B-A8A19E734225}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="33" idx="2"/>
+          <a:endCxn id="48" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7439025" y="5181600"/>
+          <a:ext cx="4763" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>122238</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>134938</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="52" name="Connector: Elbow 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64EF547F-0854-A8E4-9BA2-61585F921911}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="48" idx="2"/>
+          <a:endCxn id="3" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1">
+          <a:off x="5853113" y="4143375"/>
+          <a:ext cx="3181350" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector5">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -14671"/>
+            <a:gd name="adj2" fmla="val 13762504"/>
+            <a:gd name="adj3" fmla="val 107186"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="350096" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="TextBox 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E1A7C80-B2C4-66C2-53FA-2E013AB71BF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7124700" y="5153025"/>
+          <a:ext cx="350096" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>No</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>57151</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="59" name="Rectangle 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E84865F6-F25B-8BDA-5D81-3EFD6C0380D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8943975" y="4543425"/>
+          <a:ext cx="1476376" cy="295275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>Start new round</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>485774</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="61" name="Straight Arrow Connector 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40C20DD9-4A96-2399-2E9E-A5799A480A64}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="33" idx="3"/>
+          <a:endCxn id="59" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8410574" y="4686300"/>
+          <a:ext cx="533401" cy="4763"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>128588</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>538163</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="63" name="Connector: Elbow 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A38D507A-EAA4-07CE-BF90-B7E2CC39A7FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="59" idx="2"/>
+          <a:endCxn id="3" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1">
+          <a:off x="7419976" y="2576513"/>
+          <a:ext cx="2286000" cy="2238375"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector5">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -71667"/>
+            <a:gd name="adj2" fmla="val 199362"/>
+            <a:gd name="adj3" fmla="val 110000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>457201</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="76" name="Rectangle 75">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E00FD51C-99A4-3256-387F-452D22FEC85C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10563225" y="5229225"/>
+          <a:ext cx="1476376" cy="295275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>Player wins</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>328613</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="78" name="Straight Arrow Connector 77">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DCD1792-063D-95AF-34CF-2122C468A20B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="23" idx="2"/>
+          <a:endCxn id="76" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11287125" y="3971924"/>
+          <a:ext cx="14288" cy="1257301"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="378758" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="79" name="TextBox 78">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A335BC8-1F35-A683-72AD-72AB20882641}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11296650" y="4438650"/>
+          <a:ext cx="378758" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>Yes</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="83" name="Flowchart: Decision 82">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56B952C9-BA14-40BB-9713-15107F326D02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10429875" y="6162675"/>
+          <a:ext cx="1752600" cy="819150"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>Play again?</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>328613</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="85" name="Straight Arrow Connector 84">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92E46C36-C17C-CE08-29B5-8AB709786850}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="76" idx="2"/>
+          <a:endCxn id="83" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11301413" y="5524500"/>
+          <a:ext cx="4762" cy="638175"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="378758" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="86" name="TextBox 85">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D61FC64-E5AA-D5E5-68A1-33A2971004E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11268075" y="7000875"/>
+          <a:ext cx="378758" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>Yes</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>128587</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>188595</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="88" name="Connector: Elbow 87">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5672DE60-AA73-0600-5D73-85948F34B057}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="83" idx="2"/>
+          <a:endCxn id="2" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1">
+          <a:off x="6359366" y="2035016"/>
+          <a:ext cx="6031230" cy="3862388"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector5">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -6633"/>
+            <a:gd name="adj2" fmla="val 169421"/>
+            <a:gd name="adj3" fmla="val 103790"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>101727</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="91" name="Flowchart: Terminator 90">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED64CA23-CA0A-EB4A-AE88-5698E32BC390}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13096875" y="6848475"/>
+          <a:ext cx="914400" cy="301752"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartTerminator">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>End</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>92202</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="92" name="Flowchart: Terminator 91">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08B50587-3241-68D7-32D2-A2C55FD119C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6991350" y="171450"/>
+          <a:ext cx="914400" cy="301752"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartTerminator">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>Start</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>128587</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>92202</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>188595</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="94" name="Straight Arrow Connector 93">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3553776-A3F8-E103-F253-13C27C13648C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="92" idx="2"/>
+          <a:endCxn id="2" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7443787" y="473202"/>
+          <a:ext cx="4763" cy="477393"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>145117</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="96" name="Connector: Elbow 95">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DE532D0-D3AB-D3D1-CA69-964F70AB1D65}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="83" idx="3"/>
+          <a:endCxn id="91" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12097310" y="6572250"/>
+          <a:ext cx="1360395" cy="276225"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>128587</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>128587</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="98" name="Straight Arrow Connector 97">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59F82DF9-6647-4599-A066-FD414257B040}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="2"/>
+          <a:endCxn id="4" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7443787" y="1362075"/>
+          <a:ext cx="0" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>128587</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>128588</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="100" name="Straight Arrow Connector 99">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{054DE232-852E-72CA-BE1E-0857AB0C0352}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="2"/>
+          <a:endCxn id="3" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7443787" y="2095500"/>
+          <a:ext cx="1" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="378758" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="103" name="TextBox 102">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FDC2A81-4296-9880-112C-7FEE06DA809C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8448675" y="4438650"/>
+          <a:ext cx="378758" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>Yes</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="350096" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="104" name="TextBox 103">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09D0192A-878E-3DF7-6FF6-C0E1008147EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12306300" y="6334125"/>
+          <a:ext cx="350096" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>No</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2290,8 +4357,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{101DB607-6754-4700-AD30-CE01D69C2EB8}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z22" sqref="Z22"/>
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y12" sqref="Y12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE93360-4803-4A9F-9AEA-7E7C0DC5EF46}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>